<commit_message>
writeup draft and shifting results
</commit_message>
<xml_diff>
--- a/simplefly/bigtest/results_3.xlsx
+++ b/simplefly/bigtest/results_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellahuang/Documents/Boulder/spring '20/independent study/fireflies/simplefly/bigtest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58F1AC1-275A-D347-BA35-055DF5DE91F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9725BA60-898B-5C46-9830-DCF2C4FF3763}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="132">
   <si>
     <t>('commonsub_og', 0)</t>
   </si>
@@ -401,6 +401,21 @@
   </si>
   <si>
     <t>*fewer flashes in general…</t>
+  </si>
+  <si>
+    <t>sorted the other way</t>
+  </si>
+  <si>
+    <t>*I like!</t>
+  </si>
+  <si>
+    <t>*not bad</t>
+  </si>
+  <si>
+    <t>*pretty good</t>
+  </si>
+  <si>
+    <t>*DO SEEM MORE PERIODIC LOOKING</t>
   </si>
 </sst>
 </file>
@@ -549,7 +564,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -732,6 +747,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -896,12 +917,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1257,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,7 +1291,7 @@
     <col min="9" max="11" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1288,6 +1310,9 @@
       <c r="F1">
         <v>4.6666666666666599</v>
       </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
       <c r="H1" t="s">
         <v>70</v>
       </c>
@@ -1307,7 +1332,7 @@
         <v>6.6666666666666599</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1329,13 +1354,13 @@
       <c r="H2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="4">
@@ -1348,7 +1373,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1367,6 +1392,9 @@
       <c r="F3">
         <v>6</v>
       </c>
+      <c r="G3" t="s">
+        <v>129</v>
+      </c>
       <c r="H3" t="s">
         <v>68</v>
       </c>
@@ -1389,7 +1417,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1426,8 +1454,11 @@
       <c r="M4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1446,6 +1477,9 @@
       <c r="F5">
         <v>6.3333333333333304</v>
       </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
       <c r="H5" t="s">
         <v>82</v>
       </c>
@@ -1465,7 +1499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1503,7 +1537,7 @@
         <v>5.6666666666666599</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1522,6 +1556,9 @@
       <c r="F7">
         <v>6</v>
       </c>
+      <c r="G7" t="s">
+        <v>130</v>
+      </c>
       <c r="H7" t="s">
         <v>116</v>
       </c>
@@ -1541,7 +1578,7 @@
         <v>4.6666666666666599</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1616,7 @@
         <v>4.6666666666666599</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1617,7 +1654,7 @@
         <v>5.6666666666666599</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1655,7 +1692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1693,7 +1730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1768,7 @@
         <v>6.3333333333333304</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1769,7 +1806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1807,7 +1844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1845,7 +1882,7 @@
         <v>6.6666666666666599</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2033,6 +2070,11 @@
       </c>
       <c r="M20">
         <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>